<commit_message>
first implementation of divider
</commit_message>
<xml_diff>
--- a/Set 3 Karnaugh Tables.xlsx
+++ b/Set 3 Karnaugh Tables.xlsx
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -742,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Z41" sqref="Z41"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>